<commit_message>
All ind funcs done and integrated w/ GUI - ready for TESTS
</commit_message>
<xml_diff>
--- a/Input files/raw data/input_raw_correlations.xlsx
+++ b/Input files/raw data/input_raw_correlations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_current\NPSoftware\GitHub\Input files\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123774E7-2263-4532-851C-9EDFFEAED0F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E973F58D-D91C-4014-8D2E-C6A4D8942D96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{CA6DCBD2-6D83-47BA-9FDC-E755914F6938}"/>
+    <workbookView xWindow="120" yWindow="12" windowWidth="22920" windowHeight="12492" xr2:uid="{CA6DCBD2-6D83-47BA-9FDC-E755914F6938}"/>
   </bookViews>
   <sheets>
     <sheet name="raw data" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <dimension ref="A1:H501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>